<commit_message>
Release folder updated with latest files
</commit_message>
<xml_diff>
--- a/CRM Solution Manager/Release/CRM Configuration settings/Configuration Settings.xlsx
+++ b/CRM Solution Manager/Release/CRM Configuration settings/Configuration Settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m-jkrishnan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m-ynaresh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6149352C-86E2-473F-B163-3981BE33B724}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CE1863-3BA5-4923-A2E8-2EED6189BDB1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration Settings" sheetId="1" r:id="rId1"/>
@@ -21,16 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
-  <si>
-    <t>(Do Not Modify) Configuration Settings</t>
-  </si>
-  <si>
-    <t>(Do Not Modify) Row Checksum</t>
-  </si>
-  <si>
-    <t>(Do Not Modify) Modified On</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Configuration Key</t>
   </si>
@@ -38,15 +29,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>syed_configurationsettings:z4PhNX7vuL3xVChQ1m2AB9Yg5AULVxXcg/SpIdNs6c5H0NE8XYXysP+DGNKHfuwvY7kxvUdBeoGlODJ6+SfaPg==:syed_configurationsettingsid=%28Do%20Not%20Modify%29%20Configuration%20Settings&amp;checksumLogicalName=%28Do%20Not%20Modify%29%20Row%20Checksum&amp;modifiedon=%28Do%20Not%20Modify%29%20Modified%20On&amp;syed_name=Configuration%20Key&amp;syed_value=Value&amp;ownerid=Owner&amp;syed_description=Description</t>
-  </si>
-  <si>
     <t>BranchName</t>
   </si>
   <si>
@@ -104,7 +86,7 @@
     <t>RepositoryUrl</t>
   </si>
   <si>
-    <t>https://syamrull@dev.azure.com/syamrull/SyedAmrullahRepository/_git/SyedAmrullahRepository</t>
+    <t>https://ReachHigh@dev.azure.com/ReachHigh/DD365/_git/DD365</t>
   </si>
   <si>
     <t>SleepTimeoutInMillis</t>
@@ -153,6 +135,9 @@
   </si>
   <si>
     <t>DD365\Release\trigger.txt</t>
+  </si>
+  <si>
+    <t>syed_configurationsettings:Mxu/OBDwgnar0ngY1MBHeNx3P6KJiQGIuJwoQxX1z3SimDoUt9VknYWcszFgUTJ6y24gOvUtCkStcmvWClL8Ew==:syed_configurationsettingsid=%28Do%20Not%20Modify%29%20Configuration%20Settings&amp;checksumLogicalName=%28Do%20Not%20Modify%29%20Row%20Checksum&amp;modifiedon=%28Do%20Not%20Modify%29%20Modified%20On&amp;syed_name=Configuration%20Key&amp;syed_value=Value&amp;createdby=Created%20By&amp;modifiedby=Modified%20By</t>
   </si>
 </sst>
 </file>
@@ -185,13 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -213,16 +192,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G19" totalsRowShown="0">
-  <autoFilter ref="A1:G19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="(Do Not Modify) Configuration Settings"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="(Do Not Modify) Row Checksum"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="(Do Not Modify) Modified On"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B19" totalsRowShown="0">
+  <autoFilter ref="A1:B19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="2">
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Configuration Key"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Value"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Owner"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -526,205 +500,178 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="dataSheet"/>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="3" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="42" style="4" customWidth="1"/>
-    <col min="5" max="5" width="90.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="42" style="6" customWidth="1"/>
-    <col min="7" max="7" width="42" style="7" customWidth="1"/>
+    <col min="1" max="1" width="42" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="D2" s="8" t="s">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="D3" s="8" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="D4" s="8" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="D5" s="8" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="D6" s="8" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="D7" s="8" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="D8" s="8" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="D9" s="8" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="D10" s="8" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="D11" s="8" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="D12" s="8" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="D13" s="8" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="B16" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="D14" s="8" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="D15" s="8" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="D16" s="8" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="B19" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="4:5">
-      <c r="D17" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="4:5">
-      <c r="D18" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="4:5">
-      <c r="D19" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Date" error="(Do Not Modify) Modified On must be in the correct date and time format." promptTitle="Date and time" prompt=" " sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>1</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 100 characters long." promptTitle="Text" prompt="Maximum Length: 100 characters." sqref="D2:E1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
+  <dataValidations count="1">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 100 characters long." promptTitle="Text" prompt="Maximum Length: 100 characters." sqref="A2:B1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>100</formula1>
-    </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" error=" " promptTitle="Lookup (required)" prompt="This Owner record must already exist in Microsoft Dynamics 365 or in this source file." sqref="F2:F1048576" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 2000 characters long." promptTitle="Text" prompt="Maximum Length: 2000 characters." sqref="G2:G1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
-      <formula1>2000</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -742,11 +689,11 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>